<commit_message>
add programs' sheets to "ServerTimeEntriesByMonthAndYear" excel report
</commit_message>
<xml_diff>
--- a/GRis/Content/ExcelTemplates/ServerTimeEntriesMonthlyReportTemplate.xlsx
+++ b/GRis/Content/ExcelTemplates/ServerTimeEntriesMonthlyReportTemplate.xlsx
@@ -408,9 +408,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>